<commit_message>
edit direction VC title updated
when adding a new direction
</commit_message>
<xml_diff>
--- a/db_schema.xlsx
+++ b/db_schema.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>getUser</t>
   </si>
@@ -143,7 +143,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,6 +157,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -180,9 +187,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,18 +673,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -684,22 +693,28 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -707,42 +722,48 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="B9" t="s">
+    <row r="9" spans="1:3">
+      <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:3">
       <c r="B10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="B11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:3">
       <c r="B14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:3">
       <c r="B15" t="s">
         <v>38</v>
       </c>

</xml_diff>